<commit_message>
Add tasks, assign owner
</commit_message>
<xml_diff>
--- a/doc/WBS.xlsx
+++ b/doc/WBS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="64">
   <si>
     <t>Level1</t>
   </si>
@@ -171,6 +171,48 @@
   </si>
   <si>
     <t>String</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Park</t>
+  </si>
+  <si>
+    <t>Read String</t>
+  </si>
+  <si>
+    <t>Sorting</t>
+  </si>
+  <si>
+    <t>Searching</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>CreateGUI</t>
+  </si>
+  <si>
+    <t>GUI EventHandler</t>
+  </si>
+  <si>
+    <t>Ronnie</t>
+  </si>
+  <si>
+    <t>Joy</t>
   </si>
 </sst>
 </file>
@@ -194,7 +236,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +255,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -226,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -237,13 +285,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -560,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55:E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,31 +626,31 @@
     <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -604,7 +658,7 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -621,8 +675,8 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -631,7 +685,7 @@
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -639,159 +693,206 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="F4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
       <c r="D14" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
+      <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>27</v>
@@ -801,102 +902,153 @@
       <c r="A21" s="1">
         <v>17</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
       <c r="D21" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
-      <c r="B29" s="3"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="1" t="s">
         <v>40</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="E31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -904,106 +1056,122 @@
       <c r="A32" s="1">
         <v>28</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="5" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G32" s="3"/>
+      <c r="E32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B33" s="7"/>
       <c r="C33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G33" s="3"/>
+      <c r="E33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
-      <c r="B34" s="3"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G34" s="3"/>
+      <c r="E34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>31</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G35" s="3"/>
+      <c r="E35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>32</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="G36" s="3"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>33</v>
       </c>
-      <c r="B37" s="3"/>
+      <c r="B37" s="7"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>34</v>
       </c>
-      <c r="B38" s="3"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>35</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="A39" s="3"/>
+      <c r="B39" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>36</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="A40" s="3"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>37</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="A41" s="3"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>38</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>43</v>
@@ -1011,11 +1179,14 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>39</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>43</v>
@@ -1023,11 +1194,14 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>40</v>
-      </c>
-      <c r="B44" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="B44" s="7"/>
       <c r="C44" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>43</v>
@@ -1035,11 +1209,14 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>41</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
+      </c>
+      <c r="B45" s="7"/>
+      <c r="C45" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>43</v>
@@ -1047,11 +1224,14 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>42</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
+      </c>
+      <c r="B46" s="7"/>
+      <c r="C46" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>43</v>
@@ -1059,68 +1239,153 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
+        <v>40</v>
+      </c>
+      <c r="B47" s="7"/>
+      <c r="C47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>44</v>
-      </c>
-      <c r="B48" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="B48" s="7"/>
       <c r="C48" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>45</v>
-      </c>
-      <c r="B49" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="B49" s="7"/>
       <c r="C49" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>46</v>
-      </c>
-      <c r="B50" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="B50" s="7"/>
       <c r="C50" s="1" t="s">
-        <v>46</v>
+        <v>23</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
+        <v>44</v>
+      </c>
+      <c r="B51" s="7"/>
+      <c r="C51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>45</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>46</v>
+      </c>
+      <c r="B53" s="7"/>
+      <c r="C53" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>47</v>
+      </c>
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="7"/>
+      <c r="C56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="7"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="B42:B54"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B55:B58"/>
     <mergeCell ref="G3:G13"/>
     <mergeCell ref="C3:C14"/>
     <mergeCell ref="B2:B23"/>
     <mergeCell ref="B24:B30"/>
     <mergeCell ref="G31:G36"/>
     <mergeCell ref="B31:B38"/>
-    <mergeCell ref="B39:B51"/>
-    <mergeCell ref="C20:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Correct Merge Mistake and rollback from correct version
</commit_message>
<xml_diff>
--- a/doc/WBS.xlsx
+++ b/doc/WBS.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>Level1</t>
   </si>
@@ -216,6 +216,21 @@
   </si>
   <si>
     <t>Alan</t>
+  </si>
+  <si>
+    <t>SQL Insert</t>
+  </si>
+  <si>
+    <t>SQL Update</t>
+  </si>
+  <si>
+    <t>SQL Delete</t>
+  </si>
+  <si>
+    <t>SQL Select</t>
+  </si>
+  <si>
+    <t>SQL Order By</t>
   </si>
 </sst>
 </file>
@@ -277,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,6 +307,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -363,7 +381,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -415,7 +433,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -617,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,6 +650,7 @@
     <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -661,7 +680,7 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -678,8 +697,8 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -688,7 +707,7 @@
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -696,148 +715,148 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="7"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="7"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="1" t="s">
         <v>46</v>
       </c>
@@ -849,43 +868,43 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
+      <c r="B18" s="8"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="7"/>
+      <c r="B19" s="8"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -905,8 +924,8 @@
       <c r="A21" s="1">
         <v>17</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="1" t="s">
         <v>29</v>
       </c>
@@ -921,21 +940,21 @@
       <c r="A22" s="1">
         <v>18</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -952,7 +971,7 @@
       <c r="A25" s="1">
         <v>21</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
@@ -967,7 +986,7 @@
       <c r="A26" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="7"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="1" t="s">
         <v>10</v>
       </c>
@@ -982,7 +1001,7 @@
       <c r="A27" s="1">
         <v>23</v>
       </c>
-      <c r="B27" s="7"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
@@ -997,7 +1016,7 @@
       <c r="A28" s="1">
         <v>24</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="1" t="s">
         <v>39</v>
       </c>
@@ -1012,7 +1031,7 @@
       <c r="A29" s="1">
         <v>25</v>
       </c>
-      <c r="B29" s="7"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="1" t="s">
         <v>45</v>
       </c>
@@ -1027,7 +1046,7 @@
       <c r="A30" s="1">
         <v>26</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="1" t="s">
         <v>40</v>
       </c>
@@ -1039,99 +1058,104 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>27</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>28</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>29</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>30</v>
-      </c>
-      <c r="B34" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="B34" s="8"/>
       <c r="C34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>31</v>
-      </c>
-      <c r="B35" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="B35" s="8"/>
       <c r="C35" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="8"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
+        <v>31</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>32</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="1" t="s">
+      <c r="B37" s="8"/>
+      <c r="C37" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>33</v>
-      </c>
-      <c r="B37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>34</v>
       </c>
-      <c r="B38" s="7"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1143,252 +1167,213 @@
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
-      <c r="B40" s="7"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D40" s="3"/>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="6" t="s">
         <v>64</v>
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
-      <c r="B41" s="7"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>35</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>62</v>
+      <c r="E42" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>36</v>
-      </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>62</v>
+        <v>37</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>37</v>
-      </c>
-      <c r="B44" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="B44" s="8"/>
       <c r="C44" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>41</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>42</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>44</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>45</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>46</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>47</v>
+      </c>
+      <c r="B51" s="8"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E52" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>38</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="3" t="s">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="8"/>
+      <c r="C53" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>39</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>40</v>
-      </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>41</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>42</v>
-      </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>43</v>
-      </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>44</v>
-      </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>45</v>
-      </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>46</v>
-      </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>47</v>
-      </c>
-      <c r="B54" s="7"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="7"/>
-      <c r="C56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="7"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="7"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="8"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B42:B54"/>
+    <mergeCell ref="B42:B51"/>
     <mergeCell ref="C20:C23"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B52:B55"/>
     <mergeCell ref="G3:G13"/>
     <mergeCell ref="C3:C14"/>
     <mergeCell ref="B2:B23"/>
     <mergeCell ref="B24:B30"/>
-    <mergeCell ref="G31:G36"/>
-    <mergeCell ref="B31:B38"/>
+    <mergeCell ref="G32:G37"/>
+    <mergeCell ref="B32:B38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Connected CREATE TABLE to the File Handler Connected UPDATE, INSERT, DELETE to File Handler Implemented CommandFetch-side for WHERE and ORDERBY
</commit_message>
<xml_diff>
--- a/doc/WBS.xlsx
+++ b/doc/WBS.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="11640"/>
   </bookViews>
@@ -10,8 +10,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -236,8 +236,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,11 +319,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -627,21 +630,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
@@ -653,7 +656,7 @@
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -676,11 +679,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -693,12 +696,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -707,156 +710,156 @@
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="1" t="s">
         <v>46</v>
       </c>
@@ -864,11 +867,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="7" t="s">
         <v>48</v>
       </c>
@@ -876,35 +879,35 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+    <row r="16" spans="1:7">
+      <c r="B16" s="9"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+    <row r="17" spans="1:7">
+      <c r="B17" s="9"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>16</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -920,12 +923,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>17</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="1" t="s">
         <v>29</v>
       </c>
@@ -936,25 +939,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>18</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>19</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>20</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -967,11 +970,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>21</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
@@ -982,11 +985,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="9"/>
       <c r="C26" s="1" t="s">
         <v>10</v>
       </c>
@@ -997,11 +1000,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>23</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
@@ -1012,11 +1015,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>24</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="1" t="s">
         <v>39</v>
       </c>
@@ -1027,11 +1030,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>25</v>
       </c>
-      <c r="B29" s="8"/>
+      <c r="B29" s="9"/>
       <c r="C29" s="1" t="s">
         <v>45</v>
       </c>
@@ -1042,11 +1045,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>26</v>
       </c>
-      <c r="B30" s="8"/>
+      <c r="B30" s="9"/>
       <c r="C30" s="1" t="s">
         <v>40</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1065,11 +1068,11 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>27</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1078,84 +1081,84 @@
       <c r="E32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G32" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>28</v>
       </c>
-      <c r="B33" s="8"/>
+      <c r="B33" s="9"/>
       <c r="C33" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G33" s="8"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>29</v>
       </c>
-      <c r="B34" s="8"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>30</v>
       </c>
-      <c r="B35" s="8"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G35" s="9"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>31</v>
       </c>
-      <c r="B36" s="8"/>
+      <c r="B36" s="9"/>
       <c r="C36" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G36" s="9"/>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>32</v>
       </c>
-      <c r="B37" s="8"/>
+      <c r="B37" s="9"/>
       <c r="C37" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G37" s="9"/>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>34</v>
       </c>
-      <c r="B38" s="8"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="3"/>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="9" t="s">
         <v>58</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1167,9 +1170,9 @@
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="3"/>
-      <c r="B40" s="8"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="3" t="s">
         <v>56</v>
       </c>
@@ -1179,19 +1182,19 @@
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="3"/>
-      <c r="B41" s="8"/>
+      <c r="B41" s="9"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="1">
         <v>35</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -1204,11 +1207,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="1">
         <v>37</v>
       </c>
-      <c r="B43" s="8"/>
+      <c r="B43" s="9"/>
       <c r="C43" s="6" t="s">
         <v>16</v>
       </c>
@@ -1219,56 +1222,56 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="1">
         <v>40</v>
       </c>
-      <c r="B44" s="8"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>63</v>
+      <c r="E44" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="1">
         <v>41</v>
       </c>
-      <c r="B45" s="8"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="6" t="s">
-        <v>63</v>
+      <c r="E45" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="1">
         <v>42</v>
       </c>
-      <c r="B46" s="8"/>
+      <c r="B46" s="9"/>
       <c r="C46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>63</v>
+      <c r="E46" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>43</v>
       </c>
-      <c r="B47" s="8"/>
+      <c r="B47" s="9"/>
       <c r="C47" s="1" t="s">
         <v>23</v>
       </c>
@@ -1282,11 +1285,11 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="1">
         <v>44</v>
       </c>
-      <c r="B48" s="8"/>
+      <c r="B48" s="9"/>
       <c r="C48" s="1" t="s">
         <v>24</v>
       </c>
@@ -1297,11 +1300,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="1">
         <v>45</v>
       </c>
-      <c r="B49" s="8"/>
+      <c r="B49" s="9"/>
       <c r="C49" s="1" t="s">
         <v>25</v>
       </c>
@@ -1315,11 +1318,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="1">
         <v>46</v>
       </c>
-      <c r="B50" s="8"/>
+      <c r="B50" s="9"/>
       <c r="C50" s="1" t="s">
         <v>46</v>
       </c>
@@ -1330,14 +1333,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="1">
         <v>47</v>
       </c>
-      <c r="B51" s="8"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="8" t="s">
+      <c r="B51" s="9"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="B52" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -1347,8 +1350,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="8"/>
+    <row r="53" spans="1:8">
+      <c r="B53" s="9"/>
       <c r="C53" s="1" t="s">
         <v>61</v>
       </c>
@@ -1356,11 +1359,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="8"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="8"/>
+    <row r="54" spans="1:8">
+      <c r="B54" s="9"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="B55" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>